<commit_message>
expansão das análises automáticas
</commit_message>
<xml_diff>
--- a/analises/2023/analise_descritiva/dados/sint_resumo_por_genero_2023.xlsx
+++ b/analises/2023/analise_descritiva/dados/sint_resumo_por_genero_2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>geral_modalidade</t>
   </si>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t>max_sucesso</t>
+  </si>
+  <si>
+    <t>apoio_medio</t>
+  </si>
+  <si>
+    <t>contribuicoes</t>
+  </si>
+  <si>
+    <t>media_contribuicoes</t>
   </si>
   <si>
     <t>aon</t>
@@ -434,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -449,7 +458,7 @@
     <col min="11" max="11" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -483,13 +492,22 @@
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>44</v>
@@ -498,10 +516,10 @@
         <v>29</v>
       </c>
       <c r="E2" s="1">
-        <v>0.03295880149812734</v>
+        <v>3.295880149812734</v>
       </c>
       <c r="F2" s="1">
-        <v>0.6590909090909091</v>
+        <v>65.90909090909091</v>
       </c>
       <c r="G2" s="2">
         <v>710060.7787271431</v>
@@ -518,13 +536,22 @@
       <c r="K2" s="2">
         <v>111934.9031053756</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2">
+        <v>94.08517009767365</v>
+      </c>
+      <c r="M2">
+        <v>7547</v>
+      </c>
+      <c r="N2">
+        <v>260.2413793103448</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>117</v>
@@ -533,10 +560,10 @@
         <v>83</v>
       </c>
       <c r="E3" s="1">
-        <v>0.08764044943820225</v>
+        <v>8.764044943820224</v>
       </c>
       <c r="F3" s="1">
-        <v>0.7094017094017094</v>
+        <v>70.94017094017094</v>
       </c>
       <c r="G3" s="2">
         <v>4257136.762729836</v>
@@ -553,13 +580,22 @@
       <c r="K3" s="2">
         <v>264585.9073482947</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3">
+        <v>129.5537663642677</v>
+      </c>
+      <c r="M3">
+        <v>32860</v>
+      </c>
+      <c r="N3">
+        <v>395.9036144578313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>209</v>
@@ -568,10 +604,10 @@
         <v>140</v>
       </c>
       <c r="E4" s="1">
-        <v>0.1565543071161049</v>
+        <v>15.65543071161049</v>
       </c>
       <c r="F4" s="1">
-        <v>0.6698564593301436</v>
+        <v>66.98564593301435</v>
       </c>
       <c r="G4" s="2">
         <v>3881052.70273276</v>
@@ -588,13 +624,22 @@
       <c r="K4" s="2">
         <v>537544.5528256212</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4">
+        <v>79.80942858649695</v>
+      </c>
+      <c r="M4">
+        <v>48629</v>
+      </c>
+      <c r="N4">
+        <v>347.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>959</v>
@@ -603,10 +648,10 @@
         <v>576</v>
       </c>
       <c r="E5" s="1">
-        <v>0.7183520599250937</v>
+        <v>71.83520599250937</v>
       </c>
       <c r="F5" s="1">
-        <v>0.6006256517205423</v>
+        <v>60.06256517205423</v>
       </c>
       <c r="G5" s="2">
         <v>15212724.00148597</v>
@@ -623,13 +668,22 @@
       <c r="K5" s="2">
         <v>679297.6600721752</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5">
+        <v>87.19342470373856</v>
+      </c>
+      <c r="M5">
+        <v>174471</v>
+      </c>
+      <c r="N5">
+        <v>302.9010416666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -638,10 +692,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="1">
-        <v>0.004494382022471911</v>
+        <v>0.4494382022471911</v>
       </c>
       <c r="F6" s="1">
-        <v>0.3333333333333333</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="G6" s="2">
         <v>2305.581647320182</v>
@@ -658,13 +712,22 @@
       <c r="K6" s="2">
         <v>1720.659275370021</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6">
+        <v>50.12134015913439</v>
+      </c>
+      <c r="M6">
+        <v>46</v>
+      </c>
+      <c r="N6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>72</v>
@@ -673,10 +736,10 @@
         <v>69</v>
       </c>
       <c r="E7" s="1">
-        <v>0.04904632152588556</v>
+        <v>4.904632152588556</v>
       </c>
       <c r="F7" s="1">
-        <v>0.9583333333333334</v>
+        <v>95.83333333333334</v>
       </c>
       <c r="G7" s="2">
         <v>1479515.330087252</v>
@@ -693,13 +756,22 @@
       <c r="K7" s="2">
         <v>169836.9145144388</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7">
+        <v>95.44644410600942</v>
+      </c>
+      <c r="M7">
+        <v>15501</v>
+      </c>
+      <c r="N7">
+        <v>224.6521739130435</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>440</v>
@@ -708,10 +780,10 @@
         <v>440</v>
       </c>
       <c r="E8" s="1">
-        <v>0.2997275204359673</v>
+        <v>29.97275204359673</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G8" s="2">
         <v>9259515.000981268</v>
@@ -728,13 +800,22 @@
       <c r="K8" s="2">
         <v>708972.7845446636</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8">
+        <v>96.51058441972074</v>
+      </c>
+      <c r="M8">
+        <v>95943</v>
+      </c>
+      <c r="N8">
+        <v>218.0522727272727</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>182</v>
@@ -743,10 +824,10 @@
         <v>176</v>
       </c>
       <c r="E9" s="1">
-        <v>0.1239782016348774</v>
+        <v>12.39782016348774</v>
       </c>
       <c r="F9" s="1">
-        <v>0.967032967032967</v>
+        <v>96.7032967032967</v>
       </c>
       <c r="G9" s="2">
         <v>1145985.994178716</v>
@@ -763,13 +844,22 @@
       <c r="K9" s="2">
         <v>29736.68915792071</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9">
+        <v>66.65034280439198</v>
+      </c>
+      <c r="M9">
+        <v>17194</v>
+      </c>
+      <c r="N9">
+        <v>97.69318181818181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>763</v>
@@ -778,10 +868,10 @@
         <v>691</v>
       </c>
       <c r="E10" s="1">
-        <v>0.5197547683923706</v>
+        <v>51.97547683923705</v>
       </c>
       <c r="F10" s="1">
-        <v>0.9056356487549148</v>
+        <v>90.56356487549148</v>
       </c>
       <c r="G10" s="2">
         <v>6465887.695217357</v>
@@ -798,13 +888,22 @@
       <c r="K10" s="2">
         <v>442290.1113560894</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10">
+        <v>86.43541554443971</v>
+      </c>
+      <c r="M10">
+        <v>74806</v>
+      </c>
+      <c r="N10">
+        <v>108.2575976845152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>11</v>
@@ -813,10 +912,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="1">
-        <v>0.007493188010899182</v>
+        <v>0.7493188010899182</v>
       </c>
       <c r="F11" s="1">
-        <v>0.6363636363636364</v>
+        <v>63.63636363636363</v>
       </c>
       <c r="G11" s="2">
         <v>11227.91709450537</v>
@@ -833,13 +932,22 @@
       <c r="K11" s="2">
         <v>5515.844600589859</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11">
+        <v>55.58374799260083</v>
+      </c>
+      <c r="M11">
+        <v>202</v>
+      </c>
+      <c r="N11">
+        <v>28.85714285714286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>28</v>
@@ -848,10 +956,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="1">
-        <v>0.04093567251461988</v>
+        <v>4.093567251461988</v>
       </c>
       <c r="F12" s="1">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="G12" s="2">
         <v>1146.907757768185</v>
@@ -868,13 +976,22 @@
       <c r="K12" s="2">
         <v>353.5789934980466</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12">
+        <v>30.9975069667077</v>
+      </c>
+      <c r="M12">
+        <v>37</v>
+      </c>
+      <c r="N12">
+        <v>5.285714285714286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>9</v>
@@ -883,10 +1000,10 @@
         <v>2</v>
       </c>
       <c r="E13" s="1">
-        <v>0.0131578947368421</v>
+        <v>1.31578947368421</v>
       </c>
       <c r="F13" s="1">
-        <v>0.2222222222222222</v>
+        <v>22.22222222222222</v>
       </c>
       <c r="G13" s="2">
         <v>1022.282285906739</v>
@@ -903,13 +1020,22 @@
       <c r="K13" s="2">
         <v>538.4389998789497</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13">
+        <v>40.89129143626957</v>
+      </c>
+      <c r="M13">
+        <v>25</v>
+      </c>
+      <c r="N13">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>69</v>
@@ -918,10 +1044,10 @@
         <v>18</v>
       </c>
       <c r="E14" s="1">
-        <v>0.1008771929824561</v>
+        <v>10.08771929824561</v>
       </c>
       <c r="F14" s="1">
-        <v>0.2608695652173913</v>
+        <v>26.08695652173913</v>
       </c>
       <c r="G14" s="2">
         <v>5551.368744100646</v>
@@ -938,13 +1064,22 @@
       <c r="K14" s="2">
         <v>1753.365733305352</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14">
+        <v>18.08263434560471</v>
+      </c>
+      <c r="M14">
+        <v>307</v>
+      </c>
+      <c r="N14">
+        <v>17.05555555555556</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>101</v>
@@ -953,10 +1088,10 @@
         <v>25</v>
       </c>
       <c r="E15" s="1">
-        <v>0.1476608187134503</v>
+        <v>14.76608187134503</v>
       </c>
       <c r="F15" s="1">
-        <v>0.2475247524752475</v>
+        <v>24.75247524752475</v>
       </c>
       <c r="G15" s="2">
         <v>9304.802663330058</v>
@@ -973,13 +1108,22 @@
       <c r="K15" s="2">
         <v>2998.544454390609</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15">
+        <v>15.74416694302886</v>
+      </c>
+      <c r="M15">
+        <v>591</v>
+      </c>
+      <c r="N15">
+        <v>23.64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>477</v>
@@ -988,10 +1132,10 @@
         <v>100</v>
       </c>
       <c r="E16" s="1">
-        <v>0.6973684210526315</v>
+        <v>69.73684210526315</v>
       </c>
       <c r="F16" s="1">
-        <v>0.209643605870021</v>
+        <v>20.96436058700209</v>
       </c>
       <c r="G16" s="2">
         <v>26161.59630367918</v>
@@ -1007,6 +1151,15 @@
       </c>
       <c r="K16" s="2">
         <v>5087.076865717208</v>
+      </c>
+      <c r="L16">
+        <v>20.96281755102498</v>
+      </c>
+      <c r="M16">
+        <v>1248</v>
+      </c>
+      <c r="N16">
+        <v>12.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>